<commit_message>
Modificacion  mostrar ficha del empleado y asignacion al distributivo
</commit_message>
<xml_diff>
--- a/WebAppTH/bd.webappth.web/wwwroot/DocumentoCapacitacion/Reportados/2.xlsx
+++ b/WebAppTH/bd.webappth.web/wwwroot/DocumentoCapacitacion/Reportados/2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriano\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5911C280-0387-40A7-A765-0C4DCF7845B4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{55987F00-3E16-44F8-9A63-A520E13E514F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{6B2C13AD-1B7B-4C89-B9B9-FC5F211352C1}"/>
   </bookViews>
@@ -567,12 +567,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -897,8 +897,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.42578125" style="4"/>
-    <col min="21" max="21" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="11.42578125" style="2"/>
+    <col min="21" max="21" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -923,7 +923,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -962,7 +962,7 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="V1" t="s">
@@ -971,7 +971,7 @@
     </row>
     <row r="2" spans="1:22" ht="108" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -1030,16 +1030,16 @@
       <c r="T2" s="1">
         <v>350</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="5">
         <v>42759</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="3" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="120" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -1098,16 +1098,16 @@
       <c r="T3" s="1">
         <v>350</v>
       </c>
-      <c r="U3" s="3">
+      <c r="U3" s="5">
         <v>42823</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="3" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="132" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
@@ -1166,13 +1166,13 @@
       <c r="T4" s="1">
         <v>350</v>
       </c>
-      <c r="U4" s="3">
+      <c r="U4" s="5">
         <v>42934</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -1231,13 +1231,13 @@
       <c r="T5" s="1">
         <v>400</v>
       </c>
-      <c r="U5" s="3">
+      <c r="U5" s="5">
         <v>42954</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
@@ -1296,13 +1296,13 @@
       <c r="T6" s="1">
         <v>400</v>
       </c>
-      <c r="U6" s="3">
+      <c r="U6" s="5">
         <v>42789</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="48" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
@@ -1361,13 +1361,13 @@
       <c r="T7" s="1">
         <v>250</v>
       </c>
-      <c r="U7" s="3">
+      <c r="U7" s="5">
         <v>42782</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="48" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -1426,13 +1426,13 @@
       <c r="T8" s="1">
         <v>250</v>
       </c>
-      <c r="U8" s="3">
+      <c r="U8" s="5">
         <v>42783</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="108" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
@@ -1491,13 +1491,13 @@
       <c r="T9" s="1">
         <v>350</v>
       </c>
-      <c r="U9" s="3">
+      <c r="U9" s="5">
         <v>42759</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="132" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -1556,13 +1556,13 @@
       <c r="T10" s="1">
         <v>350</v>
       </c>
-      <c r="U10" s="3">
+      <c r="U10" s="5">
         <v>42823</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="144" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
@@ -1621,13 +1621,13 @@
       <c r="T11" s="1">
         <v>350</v>
       </c>
-      <c r="U11" s="3">
+      <c r="U11" s="5">
         <v>42823</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="108" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -1686,13 +1686,13 @@
       <c r="T12" s="1">
         <v>350</v>
       </c>
-      <c r="U12" s="3">
+      <c r="U12" s="5">
         <v>42759</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="96" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>21</v>
@@ -1751,13 +1751,13 @@
       <c r="T13" s="1">
         <v>350</v>
       </c>
-      <c r="U13" s="3">
+      <c r="U13" s="5">
         <v>42753</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>21</v>
@@ -1816,13 +1816,13 @@
       <c r="T14" s="1">
         <v>350</v>
       </c>
-      <c r="U14" s="3">
+      <c r="U14" s="5">
         <v>42850</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="96" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
@@ -1881,13 +1881,13 @@
       <c r="T15" s="1">
         <v>350</v>
       </c>
-      <c r="U15" s="3">
+      <c r="U15" s="5">
         <v>42907</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="84" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
@@ -1946,13 +1946,13 @@
       <c r="T16" s="1">
         <v>700</v>
       </c>
-      <c r="U16" s="3">
+      <c r="U16" s="5">
         <v>42990</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
@@ -2011,13 +2011,13 @@
       <c r="T17" s="1">
         <v>350</v>
       </c>
-      <c r="U17" s="3">
+      <c r="U17" s="5">
         <v>42891</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="132" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
@@ -2076,13 +2076,13 @@
       <c r="T18" s="1">
         <v>350</v>
       </c>
-      <c r="U18" s="3">
+      <c r="U18" s="5">
         <v>42766</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
@@ -2141,13 +2141,13 @@
       <c r="T19" s="1">
         <v>350</v>
       </c>
-      <c r="U19" s="3">
+      <c r="U19" s="5">
         <v>42836</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
@@ -2206,13 +2206,13 @@
       <c r="T20" s="1">
         <v>350</v>
       </c>
-      <c r="U20" s="3">
+      <c r="U20" s="5">
         <v>42786</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
@@ -2271,13 +2271,13 @@
       <c r="T21" s="1">
         <v>350</v>
       </c>
-      <c r="U21" s="3">
+      <c r="U21" s="5">
         <v>42809</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
@@ -2336,13 +2336,13 @@
       <c r="T22" s="1">
         <v>350</v>
       </c>
-      <c r="U22" s="3">
+      <c r="U22" s="5">
         <v>42845</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
@@ -2401,13 +2401,13 @@
       <c r="T23" s="1">
         <v>350</v>
       </c>
-      <c r="U23" s="3">
+      <c r="U23" s="5">
         <v>42891</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="72" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
@@ -2466,13 +2466,13 @@
       <c r="T24" s="1">
         <v>150</v>
       </c>
-      <c r="U24" s="3">
+      <c r="U24" s="5">
         <v>42935</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="96" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -2531,13 +2531,13 @@
       <c r="T25" s="1">
         <v>350</v>
       </c>
-      <c r="U25" s="3">
+      <c r="U25" s="5">
         <v>42891</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>21</v>
@@ -2596,13 +2596,13 @@
       <c r="T26" s="1">
         <v>350</v>
       </c>
-      <c r="U26" s="3">
+      <c r="U26" s="5">
         <v>42906</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>21</v>
@@ -2661,13 +2661,13 @@
       <c r="T27" s="1">
         <v>350</v>
       </c>
-      <c r="U27" s="3">
+      <c r="U27" s="5">
         <v>42956</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>21</v>
@@ -2726,13 +2726,13 @@
       <c r="T28" s="1">
         <v>350</v>
       </c>
-      <c r="U28" s="3">
+      <c r="U28" s="5">
         <v>42891</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>21</v>
@@ -2791,13 +2791,13 @@
       <c r="T29" s="1">
         <v>350</v>
       </c>
-      <c r="U29" s="3">
+      <c r="U29" s="5">
         <v>42891</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>21</v>
@@ -2856,13 +2856,13 @@
       <c r="T30" s="1">
         <v>350</v>
       </c>
-      <c r="U30" s="3">
+      <c r="U30" s="5">
         <v>42874</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="72" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>21</v>
@@ -2921,13 +2921,13 @@
       <c r="T31" s="1">
         <v>350</v>
       </c>
-      <c r="U31" s="3">
+      <c r="U31" s="5">
         <v>42957</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>21</v>
@@ -2986,13 +2986,13 @@
       <c r="T32" s="1">
         <v>350</v>
       </c>
-      <c r="U32" s="3">
+      <c r="U32" s="5">
         <v>42874</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>21</v>
@@ -3051,13 +3051,13 @@
       <c r="T33" s="1">
         <v>350</v>
       </c>
-      <c r="U33" s="3">
+      <c r="U33" s="5">
         <v>42874</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>21</v>
@@ -3116,13 +3116,13 @@
       <c r="T34" s="1">
         <v>350</v>
       </c>
-      <c r="U34" s="3">
+      <c r="U34" s="5">
         <v>42760</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="84" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>213453232</v>
+        <v>22323232</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>21</v>
@@ -3181,7 +3181,7 @@
       <c r="T35" s="1">
         <v>300</v>
       </c>
-      <c r="U35" s="3">
+      <c r="U35" s="5">
         <v>42780</v>
       </c>
     </row>

</xml_diff>